<commit_message>
minor template changes, more checkboxes and ui update
</commit_message>
<xml_diff>
--- a/Templates/mammo.xlsx
+++ b/Templates/mammo.xlsx
@@ -476,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE19BE81-1663-4E1B-9C4B-A9490BA988AF}">
   <dimension ref="A1:AG1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AG1" sqref="AG1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -485,9 +485,8 @@
     <col min="7" max="7" width="10.36328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" customWidth="1"/>
-    <col min="12" max="12" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10" customWidth="1"/>
+    <col min="13" max="13" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.1796875" bestFit="1" customWidth="1"/>
@@ -537,13 +536,13 @@
         <v>31</v>
       </c>
       <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
         <v>32</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
-      </c>
-      <c r="M1" t="s">
-        <v>8</v>
       </c>
       <c r="N1" t="s">
         <v>10</v>

</xml_diff>